<commit_message>
adding new items for alto tiete
</commit_message>
<xml_diff>
--- a/sheets/TSE.xlsx
+++ b/sheets/TSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634AD2C1-AB1A-4A55-8E52-17A237BFB543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D53B1F-22AE-47E3-9C9D-BE6D58DF64FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$55</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="289">
   <si>
     <t>731000</t>
   </si>
@@ -880,6 +880,24 @@
   </si>
   <si>
     <t>RESSUPRIMIDA LIG DE ÁGUA PDE LIVRE OP</t>
+  </si>
+  <si>
+    <t>416500</t>
+  </si>
+  <si>
+    <t>SUPRIMIDO RAMAL AGUA ABAND NÃO VISIVEL</t>
+  </si>
+  <si>
+    <t>415000</t>
+  </si>
+  <si>
+    <t>SUPRIMIDO RAMAL ANTERIOR</t>
+  </si>
+  <si>
+    <t>466500</t>
+  </si>
+  <si>
+    <t>RELIGAÇÃO DE AGUA POR SUPRESSÃO INDEV OP</t>
   </si>
 </sst>
 </file>
@@ -1301,10 +1319,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,10 +1807,10 @@
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>225</v>
+        <v>287</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>226</v>
+        <v>288</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>216</v>
@@ -1800,32 +1818,32 @@
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>131</v>
+      <c r="A46" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>131</v>
@@ -1833,10 +1851,10 @@
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>131</v>
@@ -1844,10 +1862,10 @@
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>131</v>
@@ -1855,21 +1873,21 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>160</v>
@@ -1877,10 +1895,10 @@
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>160</v>
@@ -1888,21 +1906,21 @@
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>131</v>
@@ -1910,30 +1928,36 @@
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>246</v>
+        <v>153</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
@@ -1954,6 +1978,11 @@
       <c r="A61" s="7"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1966,10 +1995,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,43 +2120,43 @@
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>131</v>
+        <v>283</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>131</v>
@@ -2135,34 +2164,56 @@
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#feat: escopo de materiais na familia de cavalete
</commit_message>
<xml_diff>
--- a/sheets/TSE.xlsx
+++ b/sheets/TSE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\Val\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D53B1F-22AE-47E3-9C9D-BE6D58DF64FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FEAFA1-F99B-4012-BE39-9F70D41F9917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,14 +24,14 @@
     <sheet name="asfalto" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$56</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="291">
   <si>
     <t>731000</t>
   </si>
@@ -898,6 +898,12 @@
   </si>
   <si>
     <t>RELIGAÇÃO DE AGUA POR SUPRESSÃO INDEV OP</t>
+  </si>
+  <si>
+    <t>472000</t>
+  </si>
+  <si>
+    <t>RESTABELECIDA LIG AGUA COM SERV ADIC</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1325,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,32 +1835,32 @@
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>227</v>
+        <v>289</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>131</v>
+      <c r="A47" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>131</v>
@@ -1862,10 +1868,10 @@
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>131</v>
@@ -1873,10 +1879,10 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>131</v>
@@ -1884,21 +1890,21 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>160</v>
@@ -1906,10 +1912,10 @@
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>160</v>
@@ -1917,21 +1923,21 @@
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>131</v>
@@ -1939,30 +1945,36 @@
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>246</v>
+        <v>153</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -1983,6 +1995,11 @@
       <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mudanças de valoração para reposição de bloquete
</commit_message>
<xml_diff>
--- a/sheets/TSE.xlsx
+++ b/sheets/TSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FEAFA1-F99B-4012-BE39-9F70D41F9917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FF5D2F-8D05-4973-B0AF-FD974E548074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="NEXEC" sheetId="3" r:id="rId3"/>
     <sheet name="invest" sheetId="4" r:id="rId4"/>
     <sheet name="retrabalho" sheetId="5" r:id="rId5"/>
-    <sheet name="n10" sheetId="6" r:id="rId6"/>
-    <sheet name="n3" sheetId="7" r:id="rId7"/>
-    <sheet name="reposicao" sheetId="8" r:id="rId8"/>
-    <sheet name="asfalto" sheetId="9" r:id="rId9"/>
+    <sheet name="n3" sheetId="7" r:id="rId6"/>
+    <sheet name="reposicao" sheetId="8" r:id="rId7"/>
+    <sheet name="asfalto" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$56</definedName>
@@ -1327,7 +1326,7 @@
   </sheetPr>
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -2557,58 +2556,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2732,15 +2686,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,12 +2869,34 @@
         <v>2</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>

<commit_message>
added poco tse and set asfalto tse proibidos
</commit_message>
<xml_diff>
--- a/sheets/TSE.xlsx
+++ b/sheets/TSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FF5D2F-8D05-4973-B0AF-FD974E548074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D26703-BD23-4E8A-A50B-97B867346925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="retrabalho" sheetId="5" r:id="rId5"/>
     <sheet name="n3" sheetId="7" r:id="rId6"/>
     <sheet name="reposicao" sheetId="8" r:id="rId7"/>
-    <sheet name="asfalto" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$56</definedName>
@@ -30,45 +29,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="291">
-  <si>
-    <t>731000</t>
-  </si>
-  <si>
-    <t>REPOSIÇÃO DE ASFALTO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="279">
   <si>
     <t>Reposicao</t>
-  </si>
-  <si>
-    <t>733000</t>
-  </si>
-  <si>
-    <t>REPOSIÇÃO DE ASFALTO INV</t>
-  </si>
-  <si>
-    <t>743000</t>
-  </si>
-  <si>
-    <t>REPOSIÇÃO DE CAPA ASFALTICA</t>
-  </si>
-  <si>
-    <t>745000</t>
-  </si>
-  <si>
-    <t>REPOSIÇÃO DE CAPA ASFALTICA INV</t>
-  </si>
-  <si>
-    <t>785000</t>
-  </si>
-  <si>
-    <t>FRESADO E RECAPEADO PAVIMENTO ASFALTICO</t>
-  </si>
-  <si>
-    <t>785500</t>
-  </si>
-  <si>
-    <t>FRESADO E RECAPEADO PAV ASFALTICO INV</t>
   </si>
   <si>
     <t>732000</t>
@@ -1339,640 +1302,640 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2026,211 +1989,211 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2256,226 +2219,226 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2503,13 +2466,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2524,7 +2487,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2536,10 +2499,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2547,7 +2510,7 @@
         <v>718100</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +2525,7 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2573,112 +2536,112 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2706,221 +2669,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2931,7 +2686,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2942,7 +2697,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2953,7 +2708,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2964,7 +2719,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2975,7 +2730,128 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missed to put 216000
</commit_message>
<xml_diff>
--- a/sheets/TSE.xlsx
+++ b/sheets/TSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irgpapais\Documents\Meus Projetos\val\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D26703-BD23-4E8A-A50B-97B867346925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06804EC-B576-47B6-98F1-20BFA7815D7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitario" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,14 @@
     <sheet name="reposicao" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">unitario!$A$3:$C$57</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="281">
   <si>
     <t>Reposicao</t>
   </si>
@@ -866,6 +866,12 @@
   </si>
   <si>
     <t>RESTABELECIDA LIG AGUA COM SERV ADIC</t>
+  </si>
+  <si>
+    <t>216000</t>
+  </si>
+  <si>
+    <t>TROCA DE HIDROMETRO PREVENTIVA AGENDADA</t>
   </si>
 </sst>
 </file>
@@ -1287,10 +1293,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,22 +1494,22 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>122</v>
+      <c r="A18" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>122</v>
@@ -1511,10 +1517,10 @@
     </row>
     <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>122</v>
@@ -1522,10 +1528,10 @@
     </row>
     <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>122</v>
@@ -1533,32 +1539,32 @@
     </row>
     <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="C22" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C23" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>122</v>
@@ -1566,10 +1572,10 @@
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>122</v>
@@ -1577,10 +1583,10 @@
     </row>
     <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>122</v>
@@ -1588,32 +1594,32 @@
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="C27" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>122</v>
@@ -1621,32 +1627,32 @@
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>148</v>
+        <v>196</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>148</v>
@@ -1654,32 +1660,32 @@
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>123</v>
+        <v>261</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>270</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>136</v>
@@ -1687,10 +1693,10 @@
     </row>
     <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>256</v>
+        <v>198</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>255</v>
+        <v>199</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>136</v>
@@ -1698,10 +1704,10 @@
     </row>
     <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>136</v>
@@ -1709,10 +1715,10 @@
     </row>
     <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>200</v>
+        <v>253</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>201</v>
+        <v>254</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>136</v>
@@ -1720,21 +1726,21 @@
     </row>
     <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>204</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>204</v>
@@ -1742,10 +1748,10 @@
     </row>
     <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>204</v>
@@ -1753,10 +1759,10 @@
     </row>
     <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>204</v>
@@ -1764,10 +1770,10 @@
     </row>
     <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>204</v>
@@ -1775,10 +1781,10 @@
     </row>
     <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>275</v>
+        <v>211</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>276</v>
+        <v>212</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>204</v>
@@ -1786,10 +1792,10 @@
     </row>
     <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>213</v>
+        <v>275</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>204</v>
@@ -1797,10 +1803,10 @@
     </row>
     <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>277</v>
+        <v>213</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>278</v>
+        <v>214</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>204</v>
@@ -1808,32 +1814,32 @@
     </row>
     <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>216</v>
+        <v>278</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>119</v>
+      <c r="A48" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>119</v>
@@ -1841,10 +1847,10 @@
     </row>
     <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>119</v>
@@ -1852,10 +1858,10 @@
     </row>
     <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>119</v>
@@ -1863,21 +1869,21 @@
     </row>
     <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>148</v>
@@ -1885,10 +1891,10 @@
     </row>
     <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>148</v>
@@ -1896,21 +1902,21 @@
     </row>
     <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>119</v>
@@ -1918,30 +1924,36 @@
     </row>
     <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>234</v>
+        <v>141</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>0</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
@@ -1962,6 +1974,11 @@
       <c r="A63" s="7"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2487,7 +2504,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>